<commit_message>
Untitled3333：Examined this question about weighted average wavelength.
</commit_message>
<xml_diff>
--- a/white-light scanning interometer/simulation/outResult.xlsx
+++ b/white-light scanning interometer/simulation/outResult.xlsx
@@ -13,7 +13,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="304">
+  <si>
+    <t>σA</t>
+  </si>
+  <si>
+    <t>Zo</t>
+  </si>
+  <si>
+    <t>λA</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>ZaT</t>
+  </si>
+  <si>
+    <t>ZpT</t>
+  </si>
+  <si>
+    <t>ZaS</t>
+  </si>
+  <si>
+    <t>ZpS</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>P - λA/2</t>
+  </si>
+  <si>
+    <t>ZaS - ZaT</t>
+  </si>
+  <si>
+    <t>ZpS - ZpT</t>
+  </si>
   <si>
     <t>σA</t>
   </si>
@@ -897,7 +945,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="109">
+  <borders count="115">
     <border>
       <left/>
       <right/>
@@ -1013,11 +1061,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1127,6 +1181,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,21 +1203,21 @@
     <col min="2" max="2" width="3.82421875" customWidth="true"/>
     <col min="3" max="3" width="12.7109375" customWidth="true"/>
     <col min="4" max="4" width="15.7109375" customWidth="true"/>
-    <col min="5" max="5" width="16.37890625" customWidth="true"/>
-    <col min="6" max="6" width="12.37890625" customWidth="true"/>
-    <col min="7" max="7" width="12.37890625" customWidth="true"/>
-    <col min="8" max="8" width="11.37890625" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2">
@@ -1173,28 +1233,28 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5">
@@ -1202,42 +1262,42 @@
         <v>35</v>
       </c>
       <c r="B5" s="0">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C5" s="0">
-        <v>1443.291843705842</v>
+        <v>-63.200008460888483</v>
       </c>
       <c r="D5" s="0">
-        <v>2.7593677844583944</v>
+        <v>0.55187355689168172</v>
       </c>
       <c r="E5" s="0">
-        <v>-104.853515625</v>
+        <v>15.029296875000005</v>
       </c>
       <c r="F5" s="0">
-        <v>-104.99718171389205</v>
+        <v>15.000563657221594</v>
       </c>
       <c r="G5" s="0">
-        <v>-104.85286458333333</v>
+        <v>15.029947916666666</v>
       </c>
       <c r="H5" s="0">
-        <v>-104.99787704249273</v>
+        <v>15.001203484584281</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8">
@@ -1245,16 +1305,16 @@
         <v>35</v>
       </c>
       <c r="B8" s="0">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="C8" s="0">
         <v>10</v>
       </c>
       <c r="D8" s="0">
-        <v>0.00065104166667140362</v>
+        <v>0.00065104166666074548</v>
       </c>
       <c r="E8" s="0">
-        <v>-0.00069532860068477476</v>
+        <v>0.00063982736268641816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>